<commit_message>
se actualizan detalles de codigo
</commit_message>
<xml_diff>
--- a/rotulos_solicitados.xlsx
+++ b/rotulos_solicitados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,143 +465,143 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>872</v>
+        <v>887</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>PENDIENTE DAV</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3650</v>
+        <v>1716</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SYNGENTA</t>
+          <t>ALESSO AGRO S.A.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Original</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>871</v>
+        <v>886</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-07-26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>FACTURADO</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>154</v>
+        <v>2200</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SYNGENTA</t>
+          <t>RURALCO SOLUCIONES S.A.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Primera</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>870</v>
+        <v>885</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-07-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>PENDIENTE</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>202</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SYNGENTA</t>
+          <t>COOP. AGR. VIDELA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Primera</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>869</v>
+        <v>884</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-07-24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>FACTURADO</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2658</v>
+        <v>1421</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SYNGENTA</t>
+          <t>MORERO Y CIA S.A</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -611,73 +611,73 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>868</v>
+        <v>883</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-07-24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>PENDIENTE</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3098</v>
+        <v>759</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SYNGENTA</t>
+          <t>MORELL VULLIEZ S.A.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Primera</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>867</v>
+        <v>882</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-06-25</t>
+          <t>2024-07-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>PENDIENTE</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>870</v>
+        <v>6009</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>COOP. ARMSTRONG</t>
+          <t>JAKAS KOKIC IVANCICH S.A.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -687,35 +687,35 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Tyveck 40KG.</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>866</v>
+        <v>881</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-07-24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>PENDIENTE DAV</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>50</v>
+        <v>13128</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SANTIAGO DUGAN TROCELLO S.R.L</t>
+          <t>COOP. CORONEL BOGADO</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Soja</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -725,26 +725,26 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Regalia</t>
+          <t>IQR</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>865</v>
+        <v>880</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-07-11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>FACTURADO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -763,35 +763,35 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Tyveck BB</t>
+          <t>Regalia</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>864</v>
+        <v>879</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-07-11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>COMPLETO</t>
+          <t>FACTURADO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2833</v>
+        <v>60</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>AFA RUEDA</t>
+          <t>SANTIAGO DUGAN TROCELLO S.R.L</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Arveja</t>
+          <t>Trigo</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -801,17 +801,17 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Tyveck 40KG.</t>
+          <t>Tyveck BB</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>863</v>
+        <v>878</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-06-19</t>
+          <t>2024-07-11</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -820,11 +820,11 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>390</v>
+        <v>15</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>COOP. VILLA CANAS</t>
+          <t>MAIOCCO CEREALES S.A.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -839,17 +839,17 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Tyveck 40KG.</t>
+          <t>Regalia</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>862</v>
+        <v>877</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-06-18</t>
+          <t>2024-07-11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -858,36 +858,36 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6400</v>
+        <v>15</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RURALCO SOLUCIONES S.A.</t>
+          <t>MAIOCCO CEREALES S.A.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Maiz</t>
+          <t>Trigo</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Hibrido</t>
+          <t>Primera</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>IQR</t>
+          <t>Tyveck BB</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>861</v>
+        <v>876</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-06-18</t>
+          <t>2024-07-10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -896,11 +896,11 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>600</v>
+        <v>2767</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>JORGE A. CASAL CEREALES S.A</t>
+          <t>MOLINO MATILDE</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -921,11 +921,11 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>860</v>
+        <v>875</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-07-10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -934,49 +934,49 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>COOP. LA PAZ LTDA</t>
+          <t>COOP. AGROP. DE LA VIOLETA</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Trigo</t>
+          <t>Arveja</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Primera</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tyveck BB</t>
+          <t>Sint. Big Bag</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>859</v>
+        <v>874</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-07-05</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FACTURADO</t>
+          <t>COMPLETO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>84</v>
+        <v>2000</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>COOP. LA PAZ LTDA</t>
+          <t>SYNGENTA</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -986,22 +986,22 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Primera</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Regalia</t>
+          <t>Otro</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>858</v>
+        <v>873</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-06-12</t>
+          <t>2024-07-04</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1010,11 +1010,11 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>58</v>
+        <v>27232</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>COOP. AGRIC. MIXTA LA PROTECTORA</t>
+          <t>MOLINO MATILDE</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1028,234 +1028,6 @@
         </is>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>Tyveck BB</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>857</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2024-06-12</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>FACTURADO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>8</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>COOP. AGRIC. MIXTA LA PROTECTORA</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Regalia</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>856</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2024-06-05</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>FACTURADO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>142</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>COOP. AGRIC. MIXTA LA PROTECTORA</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Regalia</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>855</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2024-06-05</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>FACTURADO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>242</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>COOP. AGRIC. MIXTA LA PROTECTORA</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Tyveck BB</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>854</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2024-06-04</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>FACTURADO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>72</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LA CONSTANCIA AGR S.A.</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Tyveck BB</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>853</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2024-06-04</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>COMPLETO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>13000</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>MOLINO MATILDE</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Regalia</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>852</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2024-06-04</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>FACTURADO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>750</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>COOP. VILLA CANAS</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Trigo</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Primera</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
         <is>
           <t>Tyveck 40KG.</t>
         </is>

</xml_diff>